<commit_message>
adds cancer alliance lookup and new / combined projects
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_targeted_lung_health_check/mi_data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61E99323-57CE-497A-BB86-D12260E741F8}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{404E3339-32F9-41B8-9C6B-BE6F246D9236}"/>
   <bookViews>
-    <workbookView xWindow="29355" yWindow="270" windowWidth="21315" windowHeight="15690" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="6780" yWindow="60" windowWidth="21285" windowHeight="17790" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="archive" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="122">
   <si>
     <t>Original</t>
   </si>
@@ -284,9 +288,6 @@
     <t xml:space="preserve">checked - combination of previous [Blackburn with Darwen] and [Blackpool] eligible populations </t>
   </si>
   <si>
-    <t>North East Essex and Great Yarmouth</t>
-  </si>
-  <si>
     <t>15E</t>
   </si>
   <si>
@@ -297,6 +298,114 @@
   </si>
   <si>
     <t>Blackburn Darwen and Blackpool</t>
+  </si>
+  <si>
+    <t>02Q03L</t>
+  </si>
+  <si>
+    <t>Barnsley Bassetlaw Rotherham</t>
+  </si>
+  <si>
+    <t>pop is total of three projects</t>
+  </si>
+  <si>
+    <t>NE Essex and Great Yarmouth</t>
+  </si>
+  <si>
+    <t>CACode</t>
+  </si>
+  <si>
+    <t>CAName</t>
+  </si>
+  <si>
+    <t>E56000018</t>
+  </si>
+  <si>
+    <t>Lancashire and South Cumbria</t>
+  </si>
+  <si>
+    <t>E56000024</t>
+  </si>
+  <si>
+    <t>East Midlands</t>
+  </si>
+  <si>
+    <t>E56000025</t>
+  </si>
+  <si>
+    <t>South Yorkshire and Bassetlaw</t>
+  </si>
+  <si>
+    <t>E56000026</t>
+  </si>
+  <si>
+    <t>Humber, Coast and Vale</t>
+  </si>
+  <si>
+    <t>E56000023</t>
+  </si>
+  <si>
+    <t>East of England - South</t>
+  </si>
+  <si>
+    <t>E56000029</t>
+  </si>
+  <si>
+    <t>Northern</t>
+  </si>
+  <si>
+    <t>E56000030</t>
+  </si>
+  <si>
+    <t>West Yorkshire and Harrogate</t>
+  </si>
+  <si>
+    <t>E56000016</t>
+  </si>
+  <si>
+    <t>Wessex</t>
+  </si>
+  <si>
+    <t>E56000019</t>
+  </si>
+  <si>
+    <t>Greater Manchester</t>
+  </si>
+  <si>
+    <t>E56000005</t>
+  </si>
+  <si>
+    <t>E56000007</t>
+  </si>
+  <si>
+    <t>West Midlands</t>
+  </si>
+  <si>
+    <t>E56000021</t>
+  </si>
+  <si>
+    <t>RM Partners</t>
+  </si>
+  <si>
+    <t>E56000012</t>
+  </si>
+  <si>
+    <t>Surrey and Sussex</t>
+  </si>
+  <si>
+    <t>E56000014</t>
+  </si>
+  <si>
+    <t>Peninsula</t>
+  </si>
+  <si>
+    <t>E56000028</t>
+  </si>
+  <si>
+    <t>E56000022</t>
+  </si>
+  <si>
+    <t>East of England - North</t>
   </si>
 </sst>
 </file>
@@ -361,7 +470,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -378,16 +490,53 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Project_to_CA"/>
+      <sheetName val="LU CCG to CA 2021"/>
+      <sheetName val="New CA names"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:F38" totalsRowShown="0">
-  <autoFilter ref="A1:F38" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H35" totalsRowShown="0">
+  <autoFilter ref="A1:H35" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
+  <tableColumns count="8">
     <tableColumn id="3" xr3:uid="{A5452334-59EB-4AA2-9C3A-F6252D097110}" name="project_code"/>
     <tableColumn id="1" xr3:uid="{F3A3C078-FCEE-4026-BBFD-3228BDAAD77D}" name="project"/>
     <tableColumn id="2" xr3:uid="{4B674A5C-AF2A-4FE8-A156-D3EA1935AEE0}" name="phase"/>
     <tableColumn id="4" xr3:uid="{AD6A0C7B-E6DF-40EC-9069-5EE1A0809771}" name="start_date"/>
-    <tableColumn id="5" xr3:uid="{EEAA0625-3D05-4833-BE4F-385F5E6E86C7}" name="eligible_population" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{EEAA0625-3D05-4833-BE4F-385F5E6E86C7}" name="eligible_population" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{772734CC-D9EB-4618-9C14-922AA495F6E4}" name="status"/>
+    <tableColumn id="7" xr3:uid="{FEA4EEEA-F3F0-46DB-AFD5-9B3846A01F5E}" name="CACode"/>
+    <tableColumn id="8" xr3:uid="{8846FDE2-6CCD-4719-8269-9D6F74FBB454}" name="CAName"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4B197BCF-0655-4F80-8B5C-7F7058AA2839}" name="Table13" displayName="Table13" ref="A1:F39" totalsRowShown="0">
+  <autoFilter ref="A1:F39" xr:uid="{4B197BCF-0655-4F80-8B5C-7F7058AA2839}"/>
+  <tableColumns count="6">
+    <tableColumn id="3" xr3:uid="{8E84679C-0908-428D-AE42-660B9549F56B}" name="project_code"/>
+    <tableColumn id="1" xr3:uid="{8FA097AA-96A2-437E-A811-83153EA22323}" name="project"/>
+    <tableColumn id="2" xr3:uid="{EF34FFC9-5DA6-4E08-8DAA-FA043DD42352}" name="phase"/>
+    <tableColumn id="4" xr3:uid="{ED0B2BBE-7E6B-4F34-A6AA-C53F351B1955}" name="start_date"/>
+    <tableColumn id="5" xr3:uid="{3FCB2B27-6B8F-4EF2-99D9-F4BF515622D7}" name="eligible_population" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F6D52E7E-C314-4B42-9722-7973A8896B7E}" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -682,7 +831,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -690,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,9 +853,11 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -725,13 +876,19 @@
       <c r="F1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -745,8 +902,14 @@
       <c r="F2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -765,8 +928,14 @@
       <c r="F3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -785,8 +954,14 @@
       <c r="F4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -805,8 +980,14 @@
       <c r="F5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -825,8 +1006,14 @@
       <c r="F6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -845,8 +1032,14 @@
       <c r="F7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -865,8 +1058,14 @@
       <c r="F8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -885,8 +1084,14 @@
       <c r="F9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -905,8 +1110,14 @@
       <c r="F10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -925,8 +1136,14 @@
       <c r="F11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -945,8 +1162,14 @@
       <c r="F12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -965,8 +1188,14 @@
       <c r="F13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -985,8 +1214,14 @@
       <c r="F14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1005,8 +1240,14 @@
       <c r="F15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1025,8 +1266,14 @@
       <c r="F16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1045,8 +1292,14 @@
       <c r="F17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1065,8 +1318,14 @@
       <c r="F18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1085,8 +1344,14 @@
       <c r="F19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1105,8 +1370,14 @@
       <c r="F20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1125,33 +1396,45 @@
       <c r="F21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="2">
-        <v>44774</v>
-      </c>
-      <c r="E22" s="1">
-        <v>16825</v>
+        <v>44743</v>
+      </c>
+      <c r="E22" s="5">
+        <v>30502</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="G22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -1159,39 +1442,51 @@
       <c r="D23" s="2">
         <v>44743</v>
       </c>
-      <c r="E23" s="5">
-        <v>30502</v>
+      <c r="E23" s="4">
+        <v>3682</v>
       </c>
       <c r="F23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="2">
-        <v>44743</v>
-      </c>
-      <c r="E24" s="4">
-        <v>3682</v>
+        <v>44682</v>
+      </c>
+      <c r="E24">
+        <v>49026</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -1200,118 +1495,156 @@
         <v>44682</v>
       </c>
       <c r="E25">
-        <v>49026</v>
+        <v>43868</v>
       </c>
       <c r="F25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="2">
+        <v>44743</v>
+      </c>
+      <c r="E26" s="5">
+        <v>130053</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2">
         <v>44682</v>
       </c>
-      <c r="E26">
-        <v>43868</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2">
-        <v>44743</v>
-      </c>
-      <c r="E27" s="5">
-        <v>130053</v>
+      <c r="E27">
+        <v>46093</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="2">
-        <v>44682</v>
+        <v>44652</v>
       </c>
       <c r="E28">
-        <v>46093</v>
+        <v>17543</v>
       </c>
       <c r="F28" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="2">
-        <v>44652</v>
+        <v>44835</v>
       </c>
       <c r="E29">
-        <v>17543</v>
+        <v>48186</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="2">
-        <v>44835</v>
+        <v>44774</v>
       </c>
       <c r="E30">
-        <v>48186</v>
+        <v>27000</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G30" t="str">
+        <f>_xlfn.XLOOKUP([1]!Table2[[#This Row],[Nearst CCG match]],[1]!_CA[CCG21NM],[1]!_CA[CAL21CD],0,0)</f>
+        <v>E56000015</v>
+      </c>
+      <c r="H30" t="str">
+        <f>_xlfn.XLOOKUP([1]!Table2[[#This Row],[Nearst CCG match]],[1]!_CA[CCG21NM],[1]!_CA[CAL21NM],0,0)</f>
+        <v>Somerset, Wiltshire, Avon and Gloucestershire</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -1320,18 +1653,26 @@
         <v>44774</v>
       </c>
       <c r="E31">
-        <v>27000</v>
+        <v>2300</v>
       </c>
       <c r="F31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f>_xlfn.XLOOKUP([1]!Table2[[#This Row],[Nearst CCG match]],[1]!_CA[CCG21NM],[1]!_CA[CAL21CD],0,0)</f>
+        <v>E56000015</v>
+      </c>
+      <c r="H31" t="str">
+        <f>_xlfn.XLOOKUP([1]!Table2[[#This Row],[Nearst CCG match]],[1]!_CA[CCG21NM],[1]!_CA[CAL21NM],0,0)</f>
+        <v>Somerset, Wiltshire, Avon and Gloucestershire</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -1340,127 +1681,94 @@
         <v>44774</v>
       </c>
       <c r="E32">
-        <v>2300</v>
+        <v>50000</v>
       </c>
       <c r="F32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="2">
-        <v>44774</v>
-      </c>
-      <c r="E33">
-        <v>50000</v>
+        <v>44927</v>
+      </c>
+      <c r="E33" s="1">
+        <v>14250</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="2">
-        <v>44835</v>
+        <v>44805</v>
       </c>
       <c r="E34" s="1">
-        <v>25949</v>
+        <v>48548</v>
       </c>
       <c r="F34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="2">
-        <v>44927</v>
-      </c>
-      <c r="E35" s="1">
-        <v>30348</v>
+        <v>44774</v>
+      </c>
+      <c r="E35">
+        <v>73122</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="2">
-        <v>44927</v>
-      </c>
-      <c r="E36" s="1">
-        <v>14250</v>
-      </c>
-      <c r="F36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="2">
-        <v>44805</v>
-      </c>
-      <c r="E37" s="1">
-        <v>48548</v>
-      </c>
-      <c r="F37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="2">
-        <v>44835</v>
-      </c>
-      <c r="E38" s="1">
-        <v>21315</v>
-      </c>
-      <c r="F38" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="G35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1472,6 +1780,801 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AFAB7C-FA34-498B-99C2-8625E4A5B4C2}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44256</v>
+      </c>
+      <c r="E2">
+        <v>32859</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44287</v>
+      </c>
+      <c r="E3">
+        <v>7204</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44256</v>
+      </c>
+      <c r="E4">
+        <v>37752</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>43800</v>
+      </c>
+      <c r="E5">
+        <v>26726</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44166</v>
+      </c>
+      <c r="E6">
+        <v>32333</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44256</v>
+      </c>
+      <c r="E7">
+        <v>27136</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44197</v>
+      </c>
+      <c r="E8">
+        <v>52589</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44348</v>
+      </c>
+      <c r="E9">
+        <v>20683</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43678</v>
+      </c>
+      <c r="E10">
+        <v>22109</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44348</v>
+      </c>
+      <c r="E11">
+        <v>30900</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44136</v>
+      </c>
+      <c r="E12">
+        <v>16394</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43800</v>
+      </c>
+      <c r="E13">
+        <v>27000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43556</v>
+      </c>
+      <c r="E14">
+        <v>62390</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44348</v>
+      </c>
+      <c r="E15">
+        <v>29336</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3">
+        <v>43374</v>
+      </c>
+      <c r="E16">
+        <v>7998</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>43374</v>
+      </c>
+      <c r="E17">
+        <v>22993</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>43556</v>
+      </c>
+      <c r="E18">
+        <v>20849</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2">
+        <v>43922</v>
+      </c>
+      <c r="E19">
+        <v>17117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2">
+        <v>43556</v>
+      </c>
+      <c r="E20">
+        <v>23634</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3">
+        <v>44317</v>
+      </c>
+      <c r="E21">
+        <v>19554</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2">
+        <v>44774</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16825</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2">
+        <v>44743</v>
+      </c>
+      <c r="E23" s="5">
+        <v>30502</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2">
+        <v>44743</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3682</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="2">
+        <v>44682</v>
+      </c>
+      <c r="E25">
+        <v>49026</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2">
+        <v>44682</v>
+      </c>
+      <c r="E26">
+        <v>43868</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2">
+        <v>44743</v>
+      </c>
+      <c r="E27" s="5">
+        <v>130053</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="2">
+        <v>44682</v>
+      </c>
+      <c r="E28">
+        <v>46093</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2">
+        <v>44652</v>
+      </c>
+      <c r="E29">
+        <v>17543</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2">
+        <v>44835</v>
+      </c>
+      <c r="E30">
+        <v>48186</v>
+      </c>
+      <c r="F30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="2">
+        <v>44774</v>
+      </c>
+      <c r="E31">
+        <v>27000</v>
+      </c>
+      <c r="F31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="2">
+        <v>44774</v>
+      </c>
+      <c r="E32">
+        <v>2300</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="2">
+        <v>44774</v>
+      </c>
+      <c r="E33">
+        <v>50000</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="2">
+        <v>44835</v>
+      </c>
+      <c r="E34" s="1">
+        <v>25949</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E35" s="1">
+        <v>30348</v>
+      </c>
+      <c r="F35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E36" s="1">
+        <v>14250</v>
+      </c>
+      <c r="F36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="2">
+        <v>44805</v>
+      </c>
+      <c r="E37" s="1">
+        <v>48548</v>
+      </c>
+      <c r="F37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2">
+        <v>44835</v>
+      </c>
+      <c r="E38" s="1">
+        <v>21315</v>
+      </c>
+      <c r="F38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44774</v>
+      </c>
+      <c r="E39">
+        <v>73122</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{37c354b2-85b0-47f5-b222-07b48d774ee3}" enabled="0" method="" siteId="{37c354b2-85b0-47f5-b222-07b48d774ee3}" removed="1"/>

</xml_diff>

<commit_message>
updates eligible populations for Hammersmith and Fulham and Hillingdon
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_targeted_lung_health_check/mi_data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9B7EFE7-FB04-4A30-880C-41747DC18340}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7905FE40-2A70-4C92-A0F7-A84F13EC461A}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="795" windowWidth="25995" windowHeight="16590" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="6330" yWindow="270" windowWidth="25455" windowHeight="18255" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="135">
   <si>
     <t>Original</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>E56000010</t>
+  </si>
+  <si>
+    <t>start date advised from project, pop confirmed with poppy, changed by Jane Derbyshire</t>
   </si>
 </sst>
 </file>
@@ -492,14 +495,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +858,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,10 +1277,10 @@
         <v>43374</v>
       </c>
       <c r="E16" s="1">
-        <v>23957</v>
+        <v>9630</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
         <v>113</v>
@@ -1301,10 +1303,10 @@
         <v>43374</v>
       </c>
       <c r="E17" s="1">
-        <v>9630</v>
+        <v>23957</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="G17" t="s">
         <v>113</v>
@@ -1794,7 +1796,6 @@
       <c r="D36" s="2">
         <v>44896</v>
       </c>
-      <c r="E36" s="6"/>
       <c r="F36" t="s">
         <v>128</v>
       </c>
@@ -1818,7 +1819,6 @@
       <c r="D37" s="2">
         <v>44866</v>
       </c>
-      <c r="E37" s="6"/>
       <c r="F37" t="s">
         <v>128</v>
       </c>
@@ -1842,7 +1842,6 @@
       <c r="D38" s="2">
         <v>44896</v>
       </c>
-      <c r="E38" s="6"/>
       <c r="F38" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
updates eligible population for coventry
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7905FE40-2A70-4C92-A0F7-A84F13EC461A}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14BBEC6C-9A33-4E1B-8C17-94B9970D4177}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="270" windowWidth="25455" windowHeight="18255" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="28830" yWindow="855" windowWidth="27090" windowHeight="15675" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="136">
   <si>
     <t>Original</t>
   </si>
@@ -442,6 +442,9 @@
   </si>
   <si>
     <t>start date advised from project, pop confirmed with poppy, changed by Jane Derbyshire</t>
+  </si>
+  <si>
+    <t>population advised from Karen (15/02/2023) previously using 29,336</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,11 +1253,11 @@
       <c r="D15" s="2">
         <v>44348</v>
       </c>
-      <c r="E15">
-        <v>29336</v>
+      <c r="E15" s="1">
+        <v>43650</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
adds eligible population for North Central London
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14BBEC6C-9A33-4E1B-8C17-94B9970D4177}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F3778F-C15B-466C-A034-A0E3B2D0AAFA}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="855" windowWidth="27090" windowHeight="15675" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="3870" yWindow="4470" windowWidth="27870" windowHeight="15930" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="137">
   <si>
     <t>Original</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>population advised from Karen (15/02/2023) previously using 29,336</t>
+  </si>
+  <si>
+    <t>population advised from project (2023-02-17), to check with Poppy</t>
   </si>
 </sst>
 </file>
@@ -861,7 +864,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,8 +1825,11 @@
       <c r="D37" s="2">
         <v>44866</v>
       </c>
+      <c r="E37" s="5">
+        <v>142384</v>
+      </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G37" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
added eligible population for Kent and Medway
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F3778F-C15B-466C-A034-A0E3B2D0AAFA}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFD2CD3-4366-4E8D-9236-BB3B6EF76A67}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="27870" windowHeight="15930" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="6630" yWindow="2130" windowWidth="28800" windowHeight="15990" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="138">
   <si>
     <t>Original</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>population advised from project (2023-02-17), to check with Poppy</t>
+  </si>
+  <si>
+    <t>figure from project - to check with Poppy</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,8 +1805,11 @@
       <c r="D36" s="2">
         <v>44896</v>
       </c>
+      <c r="E36" s="5">
+        <v>25662</v>
+      </c>
       <c r="F36" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="G36" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
updates eligible population estimates for a number of projects
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFD2CD3-4366-4E8D-9236-BB3B6EF76A67}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B36D825F-E5EF-432D-B523-32C05AA33BCF}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="2130" windowWidth="28800" windowHeight="15990" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="31455" yWindow="735" windowWidth="26040" windowHeight="16155" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="149">
   <si>
     <t>Original</t>
   </si>
@@ -423,9 +423,6 @@
     <t>E56000011</t>
   </si>
   <si>
-    <t>to check with Poppy</t>
-  </si>
-  <si>
     <t>North Central London</t>
   </si>
   <si>
@@ -447,10 +444,46 @@
     <t>population advised from Karen (15/02/2023) previously using 29,336</t>
   </si>
   <si>
-    <t>population advised from project (2023-02-17), to check with Poppy</t>
-  </si>
-  <si>
-    <t>figure from project - to check with Poppy</t>
+    <t>52R</t>
+  </si>
+  <si>
+    <t>Nottingham and Nottinghamshire</t>
+  </si>
+  <si>
+    <t>Dorset</t>
+  </si>
+  <si>
+    <t>11J</t>
+  </si>
+  <si>
+    <t>North and NE Lincolnshire</t>
+  </si>
+  <si>
+    <t>03H03K</t>
+  </si>
+  <si>
+    <t>Sandwell and West Birmingham</t>
+  </si>
+  <si>
+    <t>D2P2L</t>
+  </si>
+  <si>
+    <t>06/03/2023 pop from Tim Windle (previously 30502). Pop needs confirming</t>
+  </si>
+  <si>
+    <t>06/03/2023 - pop confirmed by Tim Windle. Pop needs confirming</t>
+  </si>
+  <si>
+    <t>06/03/2023 - pop from Tim Windle (previously 130053). Pop needs confirming</t>
+  </si>
+  <si>
+    <t>06/03/2023 pop confirmed by Tim Windle. figure from project - to check with Poppy</t>
+  </si>
+  <si>
+    <t>06/03/2023 pop from Tim Windle (previously 142384) population advised from project (2023-02-17), to check with Poppy</t>
+  </si>
+  <si>
+    <t>06/03/2023 pop supplied by Tim Windle</t>
   </si>
 </sst>
 </file>
@@ -466,7 +499,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +524,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -504,13 +543,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,8 +576,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H38" totalsRowShown="0">
-  <autoFilter ref="A1:H38" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H42" totalsRowShown="0">
+  <autoFilter ref="A1:H42" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
   <tableColumns count="8">
     <tableColumn id="3" xr3:uid="{A5452334-59EB-4AA2-9C3A-F6252D097110}" name="project_code"/>
     <tableColumn id="1" xr3:uid="{F3A3C078-FCEE-4026-BBFD-3228BDAAD77D}" name="project"/>
@@ -864,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1303,7 @@
         <v>43650</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
         <v>111</v>
@@ -1289,7 +1329,7 @@
         <v>9630</v>
       </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G16" t="s">
         <v>113</v>
@@ -1315,7 +1355,7 @@
         <v>23957</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
         <v>113</v>
@@ -1441,11 +1481,11 @@
       <c r="D22" s="2">
         <v>44743</v>
       </c>
-      <c r="E22" s="5">
-        <v>30502</v>
+      <c r="E22" s="6">
+        <v>44257</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="G22" t="s">
         <v>115</v>
@@ -1467,11 +1507,11 @@
       <c r="D23" s="2">
         <v>44743</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="6">
         <v>3682</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="G23" t="s">
         <v>115</v>
@@ -1545,11 +1585,11 @@
       <c r="D26" s="2">
         <v>44743</v>
       </c>
-      <c r="E26" s="5">
-        <v>130053</v>
+      <c r="E26" s="6">
+        <v>33033</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="G26" t="s">
         <v>119</v>
@@ -1805,11 +1845,11 @@
       <c r="D36" s="2">
         <v>44896</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="6">
         <v>25662</v>
       </c>
       <c r="F36" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="G36" t="s">
         <v>127</v>
@@ -1820,10 +1860,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
         <v>41</v>
@@ -1831,22 +1871,22 @@
       <c r="D37" s="2">
         <v>44866</v>
       </c>
-      <c r="E37" s="5">
-        <v>142384</v>
+      <c r="E37" s="6">
+        <v>51258</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="G37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
         <v>57</v>
@@ -1857,14 +1897,121 @@
       <c r="D38" s="2">
         <v>44896</v>
       </c>
+      <c r="E38">
+        <v>21315</v>
+      </c>
       <c r="F38" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="G38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H38" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E39">
+        <v>32118</v>
+      </c>
+      <c r="F39" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" t="s">
+        <v>94</v>
+      </c>
+      <c r="H39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E40">
+        <v>5660</v>
+      </c>
+      <c r="F40" t="s">
+        <v>148</v>
+      </c>
+      <c r="G40" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E41">
+        <v>45909</v>
+      </c>
+      <c r="F41" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" t="s">
+        <v>98</v>
+      </c>
+      <c r="H41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E42">
+        <v>34310</v>
+      </c>
+      <c r="F42" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H42" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes Luton to Luton South Bedfordshire
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/fikriyudin_mufasir_mlcsu_nhs_uk/Documents/Documents/Test_TLHC/TLHC/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD3AFA7-46D6-4497-B342-279E08A63ED0}"/>
+  <xr:revisionPtr revIDLastSave="405" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B31CDA-E1D2-49DB-BE32-EF6FD1DA9B3D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="18975" yWindow="3855" windowWidth="26040" windowHeight="17445" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="153">
   <si>
     <t>Original</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>North West and South West London</t>
+  </si>
+  <si>
+    <t>Luton South Bedfordshire</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -566,7 +569,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,23 +924,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -964,7 +966,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -990,7 +992,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1068,12 +1070,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1094,7 +1096,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1122,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1146,7 +1148,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1172,7 +1174,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1302,7 +1304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1328,7 +1330,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1380,7 +1382,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1458,7 +1460,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1562,7 +1564,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1666,7 +1668,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1718,7 +1720,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1744,7 +1746,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1848,7 +1850,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -1926,7 +1928,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>138</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -2004,7 +2006,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>142</v>
       </c>
@@ -2030,7 +2032,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>150</v>
       </c>
@@ -2043,7 +2045,6 @@
       <c r="D43" s="2">
         <v>44927</v>
       </c>
-      <c r="E43" s="7"/>
       <c r="G43" t="s">
         <v>113</v>
       </c>
@@ -2069,9 +2070,9 @@
       <selection sqref="A1:F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2151,7 +2152,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2271,7 +2272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2711,7 +2712,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>73</v>
       </c>
@@ -2768,7 +2769,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2788,7 +2789,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
Added eligible population for Hert and rename nottingham into nottingham city
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/fikriyudin_mufasir_mlcsu_nhs_uk/Documents/Documents/Test_TLHC/TLHC/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="8_{F305E0F7-7E6B-4958-8054-CF4257039E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B31CDA-E1D2-49DB-BE32-EF6FD1DA9B3D}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5FF5618-3246-4790-8B50-29BCDB4715DF}"/>
   <bookViews>
-    <workbookView xWindow="18975" yWindow="3855" windowWidth="26040" windowHeight="17445" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="156">
   <si>
     <t>Original</t>
   </si>
@@ -447,9 +447,6 @@
     <t>52R</t>
   </si>
   <si>
-    <t>Nottingham and Nottinghamshire</t>
-  </si>
-  <si>
     <t>Dorset</t>
   </si>
   <si>
@@ -496,13 +493,25 @@
   </si>
   <si>
     <t>Luton South Bedfordshire</t>
+  </si>
+  <si>
+    <t>Herts and West Essex</t>
+  </si>
+  <si>
+    <t>07H</t>
+  </si>
+  <si>
+    <t>16/03/2023 pop supplied by poppy</t>
+  </si>
+  <si>
+    <t>Nottingham City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,6 +521,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -561,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -569,6 +584,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,8 +612,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H43" totalsRowShown="0">
-  <autoFilter ref="A1:H43" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0">
+  <autoFilter ref="A1:H44" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
   <tableColumns count="8">
     <tableColumn id="3" xr3:uid="{A5452334-59EB-4AA2-9C3A-F6252D097110}" name="project_code"/>
     <tableColumn id="1" xr3:uid="{F3A3C078-FCEE-4026-BBFD-3228BDAAD77D}" name="project"/>
@@ -922,25 +940,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -966,7 +984,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -992,7 +1010,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1036,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1044,7 +1062,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1070,12 +1088,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1096,7 +1114,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1140,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1148,7 +1166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1174,7 +1192,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1226,7 +1244,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1278,7 +1296,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1304,7 +1322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1330,7 +1348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1356,7 +1374,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1382,7 +1400,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1408,7 +1426,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1434,7 +1452,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1460,7 +1478,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1486,7 +1504,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1503,7 +1521,7 @@
         <v>44257</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" t="s">
         <v>115</v>
@@ -1512,7 +1530,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1529,7 +1547,7 @@
         <v>3682</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G23" t="s">
         <v>115</v>
@@ -1538,7 +1556,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1564,7 +1582,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1590,7 +1608,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1607,7 +1625,7 @@
         <v>33033</v>
       </c>
       <c r="F26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G26" t="s">
         <v>119</v>
@@ -1616,7 +1634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1642,7 +1660,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1694,7 +1712,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1720,7 +1738,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1790,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1824,7 +1842,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1850,7 +1868,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -1867,7 +1885,7 @@
         <v>25662</v>
       </c>
       <c r="F36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G36" t="s">
         <v>127</v>
@@ -1876,7 +1894,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -1893,7 +1911,7 @@
         <v>51258</v>
       </c>
       <c r="F37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G37" t="s">
         <v>130</v>
@@ -1902,7 +1920,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -1919,7 +1937,7 @@
         <v>21315</v>
       </c>
       <c r="F38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G38" t="s">
         <v>132</v>
@@ -1928,12 +1946,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
@@ -1945,7 +1963,7 @@
         <v>32118</v>
       </c>
       <c r="F39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G39" t="s">
         <v>94</v>
@@ -1954,12 +1972,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
@@ -1971,7 +1989,7 @@
         <v>5660</v>
       </c>
       <c r="F40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G40" t="s">
         <v>106</v>
@@ -1980,12 +1998,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -1997,7 +2015,7 @@
         <v>45909</v>
       </c>
       <c r="F41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G41" t="s">
         <v>98</v>
@@ -2006,12 +2024,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
@@ -2023,7 +2041,7 @@
         <v>34310</v>
       </c>
       <c r="F42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G42" t="s">
         <v>111</v>
@@ -2032,12 +2050,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
@@ -2049,7 +2067,33 @@
         <v>113</v>
       </c>
       <c r="H43" t="s">
-        <v>151</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="2">
+        <v>44866</v>
+      </c>
+      <c r="E44">
+        <v>800</v>
+      </c>
+      <c r="F44" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" t="s">
+        <v>100</v>
+      </c>
+      <c r="H44" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2070,9 +2114,9 @@
       <selection sqref="A1:F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2092,7 +2136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2112,7 +2156,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2152,7 +2196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2172,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2192,7 +2236,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2212,7 +2256,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2276,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2252,7 +2296,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2272,7 +2316,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2292,7 +2336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2356,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2332,7 +2376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2352,7 +2396,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2372,7 +2416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2392,7 +2436,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2412,7 +2456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2452,7 +2496,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2472,7 +2516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2492,7 +2536,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2512,7 +2556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2532,7 +2576,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2552,7 +2596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2572,7 +2616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2592,7 +2636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2612,7 +2656,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2632,7 +2676,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2652,7 +2696,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2672,7 +2716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2692,7 +2736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2712,7 +2756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2732,7 +2776,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2752,7 +2796,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>73</v>
       </c>
@@ -2769,7 +2813,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2789,7 +2833,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2809,7 +2853,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -2829,7 +2873,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
corrects swindons eligible population estimate to 23000
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/fikriyudin_mufasir_mlcsu_nhs_uk/Documents/Documents/Test_TLHC/TLHC/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5FF5618-3246-4790-8B50-29BCDB4715DF}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AF6A61D-8DAC-4C54-B2E1-EC864F4169EE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="24300" windowHeight="16905" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -943,22 +943,22 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="104.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -984,7 +984,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>44774</v>
       </c>
       <c r="E31">
-        <v>2300</v>
+        <v>23000</v>
       </c>
       <c r="F31" t="s">
         <v>75</v>
@@ -1764,7 +1764,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -2114,9 +2114,9 @@
       <selection sqref="A1:F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>73</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
corrects swindon's cancer alliance to be thames valley
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AF6A61D-8DAC-4C54-B2E1-EC864F4169EE}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CCFBE2-F10B-4475-9724-500837DB3044}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="24300" windowHeight="16905" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="27135" windowHeight="17595" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="159">
   <si>
     <t>Original</t>
   </si>
@@ -505,6 +505,15 @@
   </si>
   <si>
     <t>Nottingham City</t>
+  </si>
+  <si>
+    <t>E56000013</t>
+  </si>
+  <si>
+    <t>Thames Valley</t>
+  </si>
+  <si>
+    <t>checked - corrected from previous 2300</t>
   </si>
 </sst>
 </file>
@@ -943,7 +952,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,13 +1764,13 @@
         <v>23000</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="G31" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="H31" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
corrects portsmouth's eligible popultion
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CCFBE2-F10B-4475-9724-500837DB3044}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F203875-3101-40A4-9851-C6C37792EACE}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="27135" windowHeight="17595" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="28950" yWindow="15" windowWidth="27165" windowHeight="16125" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="160">
   <si>
     <t>Original</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>checked - corrected from previous 2300</t>
+  </si>
+  <si>
+    <t>21/04/2023 pop set to 23924 (previously 46,093 - unknown where this figure was derived)</t>
   </si>
 </sst>
 </file>
@@ -951,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,10 +1660,10 @@
         <v>44682</v>
       </c>
       <c r="E27">
-        <v>46093</v>
+        <v>23924</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="G27" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
added 2 project (Hounslow and Wandsworth) from RM partners and changed eligible population for Bsol
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/fikriyudin_mufasir_mlcsu_nhs_uk/Documents/Documents/Test_TLHC/TLHC/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F203875-3101-40A4-9851-C6C37792EACE}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AE972B-6473-425D-A953-A03DA442D6BD}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="15" windowWidth="27165" windowHeight="16125" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="165">
   <si>
     <t>Original</t>
   </si>
@@ -517,6 +517,21 @@
   </si>
   <si>
     <t>21/04/2023 pop set to 23924 (previously 46,093 - unknown where this figure was derived)</t>
+  </si>
+  <si>
+    <t>08X</t>
+  </si>
+  <si>
+    <t>Wandsworth</t>
+  </si>
+  <si>
+    <t>07Y</t>
+  </si>
+  <si>
+    <t>Hounslow</t>
+  </si>
+  <si>
+    <t>18/05/2023 Tim Windle agreed to change from 48548 to 21847</t>
   </si>
 </sst>
 </file>
@@ -576,7 +591,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -584,11 +599,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -599,6 +682,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,10 +1939,10 @@
         <v>44805</v>
       </c>
       <c r="E34" s="1">
-        <v>48548</v>
+        <v>21847</v>
       </c>
       <c r="F34" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="G34" t="s">
         <v>111</v>
@@ -2106,6 +2203,50 @@
       </c>
       <c r="H44" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="12">
+        <v>45047</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="16">
+        <v>45047</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates NG eligible population based on feedback
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/fikriyudin_mufasir_mlcsu_nhs_uk/Documents/Documents/Test_TLHC/TLHC/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AE972B-6473-425D-A953-A03DA442D6BD}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10758AAD-37DC-474C-BEDD-DB0944045C3C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="32985" windowHeight="16980" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="166">
   <si>
     <t>Original</t>
   </si>
@@ -532,6 +532,9 @@
   </si>
   <si>
     <t>18/05/2023 Tim Windle agreed to change from 48548 to 21847</t>
+  </si>
+  <si>
+    <t>population advised from Vicky Cunningham (21/06/2023) previously 52,589</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -682,20 +685,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,10 +1263,10 @@
         <v>44197</v>
       </c>
       <c r="E8">
-        <v>52589</v>
+        <v>46908</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="G8" t="s">
         <v>102</v>
@@ -2205,47 +2205,47 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="12">
+      <c r="C45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="11">
         <v>45047</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="13" t="s">
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H45" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="C46" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="14">
         <v>45047</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="17" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="15" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates projects with additional characteristics from the recent ipsos / nhse review
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10758AAD-37DC-474C-BEDD-DB0944045C3C}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37094577-9C53-410C-AF53-825F78CFB568}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="32985" windowHeight="16980" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="1230" yWindow="795" windowWidth="43200" windowHeight="17235" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={60FE0030-A439-4052-8FCE-195FF2F5D4EF}</author>
+    <author>tc={FF25F602-B3A1-488E-BDC8-8184D55A62BB}</author>
+    <author>tc={23907AAF-FB2D-48E1-8D70-A9826A424DB0}</author>
+    <author>tc={4088AA37-9A7A-4B11-974A-D8E53ABA933B}</author>
+    <author>tc={5E69B891-4EB7-4137-9374-F503E28CE7B9}</author>
+    <author>tc={4B978997-F8F0-46FD-B19F-FCD562CC30DD}</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{60FE0030-A439-4052-8FCE-195FF2F5D4EF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' project delivery models doc 221205
+Reply:
+    Updated in Nov 2023 and kept as reference</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{FF25F602-B3A1-488E-BDC8-8184D55A62BB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' project delivery models doc 221205 and updated for phase 1 and 2 projects from Ipsos' 'project delivery models for 'Jan23 report'</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="2" shapeId="0" xr:uid="{23907AAF-FB2D-48E1-8D70-A9826A424DB0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' project delivery models doc 221205
+Reply:
+    Updated in Nov 2023 and kept as reference</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="3" shapeId="0" xr:uid="{4088AA37-9A7A-4B11-974A-D8E53ABA933B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' project delivery models doc 221205 and updated for phase 1 and 2 projects from Ipsos' 'project delivery models for 'Jan23 report'</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="4" shapeId="0" xr:uid="{5E69B891-4EB7-4137-9374-F503E28CE7B9}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' 'project delivery models for 'Jan23 report'
+</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="5" shapeId="0" xr:uid="{4B978997-F8F0-46FD-B19F-FCD562CC30DD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Taken from Ipsos' 'project delivery models for 'Jan23 report'</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="185">
   <si>
     <t>Original</t>
   </si>
@@ -535,13 +603,70 @@
   </si>
   <si>
     <t>population advised from Vicky Cunningham (21/06/2023) previously 52,589</t>
+  </si>
+  <si>
+    <t>invite_mode</t>
+  </si>
+  <si>
+    <t>Opt-in</t>
+  </si>
+  <si>
+    <t>Opt-out</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>lhc_delivery</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t>F2F</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Face-to-face</t>
+  </si>
+  <si>
+    <t>invite_mode_old</t>
+  </si>
+  <si>
+    <t>lhc_delivery_old</t>
+  </si>
+  <si>
+    <t>ct_scan_location</t>
+  </si>
+  <si>
+    <t>triage_before_risk_assessment</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Acute</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,8 +686,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,8 +725,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -602,79 +740,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -685,24 +755,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -720,18 +824,30 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="PARYLO, Craig (NHS MIDLANDS AND LANCASHIRE COMMISSIONING SUPPORT UNIT)" id="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" userId="S::craig.parylo2@nhs.net::975a189f-717d-4b0b-bfaf-8e8244fbf75a" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0">
-  <autoFilter ref="A1:H44" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:N46" totalsRowShown="0">
+  <autoFilter ref="A1:N46" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
+  <tableColumns count="14">
     <tableColumn id="3" xr3:uid="{A5452334-59EB-4AA2-9C3A-F6252D097110}" name="project_code"/>
     <tableColumn id="1" xr3:uid="{F3A3C078-FCEE-4026-BBFD-3228BDAAD77D}" name="project"/>
     <tableColumn id="2" xr3:uid="{4B674A5C-AF2A-4FE8-A156-D3EA1935AEE0}" name="phase"/>
     <tableColumn id="4" xr3:uid="{AD6A0C7B-E6DF-40EC-9069-5EE1A0809771}" name="start_date"/>
-    <tableColumn id="5" xr3:uid="{EEAA0625-3D05-4833-BE4F-385F5E6E86C7}" name="eligible_population" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{EEAA0625-3D05-4833-BE4F-385F5E6E86C7}" name="eligible_population" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{772734CC-D9EB-4618-9C14-922AA495F6E4}" name="status"/>
     <tableColumn id="7" xr3:uid="{FEA4EEEA-F3F0-46DB-AFD5-9B3846A01F5E}" name="CACode"/>
     <tableColumn id="8" xr3:uid="{8846FDE2-6CCD-4719-8269-9D6F74FBB454}" name="CAName"/>
+    <tableColumn id="9" xr3:uid="{E658B9EA-4FC4-453D-A322-F0C514C72A96}" name="invite_mode_old" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{52CD3B52-F138-4C9A-8B82-860E017C02DB}" name="invite_mode"/>
+    <tableColumn id="10" xr3:uid="{920BD06A-E959-4B1A-8B06-2E2F09986076}" name="lhc_delivery_old" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{7FFE1B9F-71C0-4EFD-A21C-27202A0B7BF1}" name="lhc_delivery"/>
+    <tableColumn id="13" xr3:uid="{C2434813-1622-4A19-96FE-56285A9DB982}" name="ct_scan_location"/>
+    <tableColumn id="14" xr3:uid="{2A6734E7-5839-45EC-BA19-D9414D769BD8}" name="triage_before_risk_assessment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,12 +1163,42 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I1" dT="2023-07-03T10:36:41.88" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{60FE0030-A439-4052-8FCE-195FF2F5D4EF}">
+    <text>Taken from Ipsos' project delivery models doc 221205</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2023-11-10T14:12:33.01" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{1028145C-271D-4F71-93A3-8641E87B7C0D}" parentId="{60FE0030-A439-4052-8FCE-195FF2F5D4EF}">
+    <text>Updated in Nov 2023 and kept as reference</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2023-11-10T13:54:25.95" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{FF25F602-B3A1-488E-BDC8-8184D55A62BB}">
+    <text>Taken from Ipsos' project delivery models doc 221205 and updated for phase 1 and 2 projects from Ipsos' 'project delivery models for 'Jan23 report'</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2023-07-03T10:36:51.28" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{23907AAF-FB2D-48E1-8D70-A9826A424DB0}">
+    <text>Taken from Ipsos' project delivery models doc 221205</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2023-11-10T14:12:43.12" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{EEC2B73C-7464-4450-A8CF-9FD957214FB8}" parentId="{23907AAF-FB2D-48E1-8D70-A9826A424DB0}">
+    <text>Updated in Nov 2023 and kept as reference</text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2023-11-10T14:02:16.12" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{4088AA37-9A7A-4B11-974A-D8E53ABA933B}">
+    <text>Taken from Ipsos' project delivery models doc 221205 and updated for phase 1 and 2 projects from Ipsos' 'project delivery models for 'Jan23 report'</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2023-11-10T14:04:31.58" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{5E69B891-4EB7-4137-9374-F503E28CE7B9}">
+    <text xml:space="preserve">Taken from Ipsos' 'project delivery models for 'Jan23 report'
+</text>
+  </threadedComment>
+  <threadedComment ref="N1" dT="2023-11-10T14:04:50.22" personId="{B526FAA2-A343-419A-9C55-9E73C5BAC9B3}" id="{4B978997-F8F0-46FD-B19F-FCD562CC30DD}">
+    <text>Taken from Ipsos' 'project delivery models for 'Jan23 report'</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:H46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,9 +1211,15 @@
     <col min="6" max="6" width="104.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1092,8 +1244,26 @@
       <c r="H1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1118,8 +1288,26 @@
       <c r="H2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1144,8 +1332,26 @@
       <c r="H3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J3" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1170,8 +1376,26 @@
       <c r="H4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" t="s">
+        <v>172</v>
+      </c>
+      <c r="M4" t="s">
+        <v>180</v>
+      </c>
+      <c r="N4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1196,8 +1420,26 @@
       <c r="H5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" t="s">
+        <v>172</v>
+      </c>
+      <c r="M5" t="s">
+        <v>180</v>
+      </c>
+      <c r="N5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1222,8 +1464,26 @@
       <c r="H6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J6" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L6" t="s">
+        <v>172</v>
+      </c>
+      <c r="M6" t="s">
+        <v>180</v>
+      </c>
+      <c r="N6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1248,8 +1508,26 @@
       <c r="H7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M7" t="s">
+        <v>180</v>
+      </c>
+      <c r="N7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1274,8 +1552,26 @@
       <c r="H8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L8" t="s">
+        <v>172</v>
+      </c>
+      <c r="M8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1300,8 +1596,26 @@
       <c r="H9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L9" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" t="s">
+        <v>180</v>
+      </c>
+      <c r="N9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1326,8 +1640,26 @@
       <c r="H10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L10" t="s">
+        <v>174</v>
+      </c>
+      <c r="M10" t="s">
+        <v>180</v>
+      </c>
+      <c r="N10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1352,8 +1684,26 @@
       <c r="H11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" t="s">
+        <v>169</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L11" t="s">
+        <v>175</v>
+      </c>
+      <c r="M11" t="s">
+        <v>180</v>
+      </c>
+      <c r="N11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1378,8 +1728,26 @@
       <c r="H12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" t="s">
+        <v>169</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L12" t="s">
+        <v>172</v>
+      </c>
+      <c r="M12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1404,8 +1772,26 @@
       <c r="H13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" t="s">
+        <v>172</v>
+      </c>
+      <c r="M13" t="s">
+        <v>180</v>
+      </c>
+      <c r="N13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1430,8 +1816,26 @@
       <c r="H14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" t="s">
+        <v>169</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L14" t="s">
+        <v>172</v>
+      </c>
+      <c r="M14" t="s">
+        <v>181</v>
+      </c>
+      <c r="N14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1456,8 +1860,26 @@
       <c r="H15" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" t="s">
+        <v>169</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L15" t="s">
+        <v>174</v>
+      </c>
+      <c r="M15" t="s">
+        <v>180</v>
+      </c>
+      <c r="N15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1482,8 +1904,26 @@
       <c r="H16" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" t="s">
+        <v>167</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L16" t="s">
+        <v>172</v>
+      </c>
+      <c r="M16" t="s">
+        <v>182</v>
+      </c>
+      <c r="N16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1508,8 +1948,26 @@
       <c r="H17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" t="s">
+        <v>167</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L17" t="s">
+        <v>172</v>
+      </c>
+      <c r="M17" t="s">
+        <v>180</v>
+      </c>
+      <c r="N17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1534,8 +1992,26 @@
       <c r="H18" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" t="s">
+        <v>169</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L18" t="s">
+        <v>175</v>
+      </c>
+      <c r="M18" t="s">
+        <v>180</v>
+      </c>
+      <c r="N18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1560,8 +2036,26 @@
       <c r="H19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J19" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L19" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" t="s">
+        <v>182</v>
+      </c>
+      <c r="N19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1586,8 +2080,26 @@
       <c r="H20" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" t="s">
+        <v>168</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L20" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" t="s">
+        <v>182</v>
+      </c>
+      <c r="N20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1612,8 +2124,26 @@
       <c r="H21" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J21" t="s">
+        <v>167</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L21" t="s">
+        <v>172</v>
+      </c>
+      <c r="M21" t="s">
+        <v>180</v>
+      </c>
+      <c r="N21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1638,8 +2168,26 @@
       <c r="H22" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J22" t="s">
+        <v>169</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L22" t="s">
+        <v>172</v>
+      </c>
+      <c r="M22" t="s">
+        <v>170</v>
+      </c>
+      <c r="N22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1664,8 +2212,26 @@
       <c r="H23" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J23" t="s">
+        <v>169</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L23" t="s">
+        <v>172</v>
+      </c>
+      <c r="M23" t="s">
+        <v>170</v>
+      </c>
+      <c r="N23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1690,8 +2256,26 @@
       <c r="H24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L24" t="s">
+        <v>172</v>
+      </c>
+      <c r="M24" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1716,8 +2300,26 @@
       <c r="H25" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" t="s">
+        <v>169</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L25" t="s">
+        <v>172</v>
+      </c>
+      <c r="M25" t="s">
+        <v>170</v>
+      </c>
+      <c r="N25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1742,8 +2344,26 @@
       <c r="H26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L26" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" t="s">
+        <v>170</v>
+      </c>
+      <c r="N26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1768,8 +2388,26 @@
       <c r="H27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" t="s">
+        <v>169</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L27" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" t="s">
+        <v>170</v>
+      </c>
+      <c r="N27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1794,8 +2432,26 @@
       <c r="H28" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" t="s">
+        <v>169</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L28" t="s">
+        <v>172</v>
+      </c>
+      <c r="M28" t="s">
+        <v>170</v>
+      </c>
+      <c r="N28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1820,8 +2476,26 @@
       <c r="H29" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J29" t="s">
+        <v>170</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L29" t="s">
+        <v>170</v>
+      </c>
+      <c r="M29" t="s">
+        <v>170</v>
+      </c>
+      <c r="N29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1846,8 +2520,26 @@
       <c r="H30" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" t="s">
+        <v>169</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L30" t="s">
+        <v>172</v>
+      </c>
+      <c r="M30" t="s">
+        <v>170</v>
+      </c>
+      <c r="N30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1872,8 +2564,26 @@
       <c r="H31" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L31" t="s">
+        <v>172</v>
+      </c>
+      <c r="M31" t="s">
+        <v>170</v>
+      </c>
+      <c r="N31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1898,8 +2608,26 @@
       <c r="H32" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J32" t="s">
+        <v>169</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L32" t="s">
+        <v>172</v>
+      </c>
+      <c r="M32" t="s">
+        <v>170</v>
+      </c>
+      <c r="N32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1924,8 +2652,26 @@
       <c r="H33" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J33" t="s">
+        <v>170</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L33" t="s">
+        <v>170</v>
+      </c>
+      <c r="M33" t="s">
+        <v>170</v>
+      </c>
+      <c r="N33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1950,8 +2696,26 @@
       <c r="H34" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J34" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L34" t="s">
+        <v>170</v>
+      </c>
+      <c r="M34" t="s">
+        <v>170</v>
+      </c>
+      <c r="N34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1976,8 +2740,26 @@
       <c r="H35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J35" t="s">
+        <v>168</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L35" t="s">
+        <v>172</v>
+      </c>
+      <c r="M35" t="s">
+        <v>170</v>
+      </c>
+      <c r="N35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -2002,8 +2784,26 @@
       <c r="H36" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J36" t="s">
+        <v>170</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L36" t="s">
+        <v>170</v>
+      </c>
+      <c r="M36" t="s">
+        <v>170</v>
+      </c>
+      <c r="N36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -2028,8 +2828,26 @@
       <c r="H37" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J37" t="s">
+        <v>170</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L37" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37" t="s">
+        <v>170</v>
+      </c>
+      <c r="N37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -2054,8 +2872,26 @@
       <c r="H38" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J38" t="s">
+        <v>170</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L38" t="s">
+        <v>170</v>
+      </c>
+      <c r="M38" t="s">
+        <v>170</v>
+      </c>
+      <c r="N38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -2080,8 +2916,26 @@
       <c r="H39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J39" t="s">
+        <v>170</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L39" t="s">
+        <v>170</v>
+      </c>
+      <c r="M39" t="s">
+        <v>170</v>
+      </c>
+      <c r="N39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -2106,8 +2960,26 @@
       <c r="H40" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J40" t="s">
+        <v>170</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L40" t="s">
+        <v>170</v>
+      </c>
+      <c r="M40" t="s">
+        <v>170</v>
+      </c>
+      <c r="N40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -2132,8 +3004,26 @@
       <c r="H41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J41" t="s">
+        <v>170</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L41" t="s">
+        <v>170</v>
+      </c>
+      <c r="M41" t="s">
+        <v>170</v>
+      </c>
+      <c r="N41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -2158,8 +3048,26 @@
       <c r="H42" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J42" t="s">
+        <v>170</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L42" t="s">
+        <v>170</v>
+      </c>
+      <c r="M42" t="s">
+        <v>170</v>
+      </c>
+      <c r="N42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -2178,8 +3086,26 @@
       <c r="H43" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J43" t="s">
+        <v>170</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L43" t="s">
+        <v>170</v>
+      </c>
+      <c r="M43" t="s">
+        <v>170</v>
+      </c>
+      <c r="N43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -2204,57 +3130,108 @@
       <c r="H44" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="I44" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J44" t="s">
+        <v>170</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L44" t="s">
+        <v>170</v>
+      </c>
+      <c r="M44" t="s">
+        <v>170</v>
+      </c>
+      <c r="N44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="11">
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="2">
         <v>45047</v>
       </c>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10" t="s">
+      <c r="G45" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="I45" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J45" t="s">
+        <v>170</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L45" t="s">
+        <v>170</v>
+      </c>
+      <c r="M45" t="s">
+        <v>170</v>
+      </c>
+      <c r="N45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>162</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="14">
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="2">
         <v>45047</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13" t="s">
+      <c r="G46" t="s">
         <v>113</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="H46" t="s">
         <v>114</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" t="s">
+        <v>170</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L46" t="s">
+        <v>170</v>
+      </c>
+      <c r="M46" t="s">
+        <v>170</v>
+      </c>
+      <c r="N46" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adds admin category to project lookup
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37094577-9C53-410C-AF53-825F78CFB568}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F2B714-A951-4D70-9D97-11F8BA170849}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="795" windowWidth="43200" windowHeight="17235" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="16395" yWindow="11190" windowWidth="30945" windowHeight="10530" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="188">
   <si>
     <t>Original</t>
   </si>
@@ -660,6 +660,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Outsourced</t>
+  </si>
+  <si>
+    <t>In-house</t>
   </si>
 </sst>
 </file>
@@ -831,9 +840,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:N46" totalsRowShown="0">
-  <autoFilter ref="A1:N46" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}" name="Table1" displayName="Table1" ref="A1:O46" totalsRowShown="0">
+  <autoFilter ref="A1:O46" xr:uid="{97CCC447-797C-486E-85C3-976D61CFF28E}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Onboarded"/>
+        <filter val="Original"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="15">
     <tableColumn id="3" xr3:uid="{A5452334-59EB-4AA2-9C3A-F6252D097110}" name="project_code"/>
     <tableColumn id="1" xr3:uid="{F3A3C078-FCEE-4026-BBFD-3228BDAAD77D}" name="project"/>
     <tableColumn id="2" xr3:uid="{4B674A5C-AF2A-4FE8-A156-D3EA1935AEE0}" name="phase"/>
@@ -848,6 +864,7 @@
     <tableColumn id="12" xr3:uid="{7FFE1B9F-71C0-4EFD-A21C-27202A0B7BF1}" name="lhc_delivery"/>
     <tableColumn id="13" xr3:uid="{C2434813-1622-4A19-96FE-56285A9DB982}" name="ct_scan_location"/>
     <tableColumn id="14" xr3:uid="{2A6734E7-5839-45EC-BA19-D9414D769BD8}" name="triage_before_risk_assessment"/>
+    <tableColumn id="15" xr3:uid="{8C36AD16-0570-4B1C-A6A3-14FFCDEE628F}" name="admin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1195,31 +1212,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="104.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1262,8 +1280,11 @@
       <c r="N1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1306,8 +1327,11 @@
       <c r="N2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1350,8 +1374,11 @@
       <c r="N3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1394,8 +1421,11 @@
       <c r="N4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1438,8 +1468,11 @@
       <c r="N5" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1482,8 +1515,11 @@
       <c r="N6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1526,8 +1562,11 @@
       <c r="N7" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1570,8 +1609,11 @@
       <c r="N8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1614,8 +1656,11 @@
       <c r="N9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1658,8 +1703,11 @@
       <c r="N10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1702,8 +1750,11 @@
       <c r="N11" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1746,8 +1797,11 @@
       <c r="N12" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1790,8 +1844,11 @@
       <c r="N13" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1834,8 +1891,11 @@
       <c r="N14" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1878,8 +1938,11 @@
       <c r="N15" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1922,8 +1985,11 @@
       <c r="N16" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1966,8 +2032,11 @@
       <c r="N17" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2010,8 +2079,11 @@
       <c r="N18" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2054,8 +2126,11 @@
       <c r="N19" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2098,8 +2173,11 @@
       <c r="N20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2142,8 +2220,11 @@
       <c r="N21" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2187,7 +2268,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2231,7 +2312,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2275,7 +2356,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2319,7 +2400,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2363,7 +2444,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2407,7 +2488,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2451,7 +2532,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2495,7 +2576,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -2539,7 +2620,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -2583,7 +2664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2627,7 +2708,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2671,7 +2752,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2715,7 +2796,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2759,7 +2840,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -2803,7 +2884,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -2847,7 +2928,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -2891,7 +2972,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -2935,7 +3016,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -2979,7 +3060,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -3023,7 +3104,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -3067,7 +3148,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -3105,7 +3186,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -3149,7 +3230,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>160</v>
       </c>
@@ -3187,7 +3268,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
updates the project reference file
</commit_message>
<xml_diff>
--- a/data/reference/project_reference.xlsx
+++ b/data/reference/project_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc_new/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F2B714-A951-4D70-9D97-11F8BA170849}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="114_{44416DCD-0D48-48A0-9934-02FA0A67BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CE9C39-F71D-4057-AFE5-1FA176C8A8E0}"/>
   <bookViews>
-    <workbookView xWindow="16395" yWindow="11190" windowWidth="30945" windowHeight="10530" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
+    <workbookView xWindow="6495" yWindow="10740" windowWidth="20715" windowHeight="12540" xr2:uid="{21102F19-DBE8-4D92-B721-B3924BFAE080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -886,9 +886,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -926,7 +926,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1032,7 +1032,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1174,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9290F322-6BDD-49FD-ACC8-5115825FDB32}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>